<commit_message>
will work on the stock details next. On this one I deleted Manager, Owner and all related repository,service, and the controller classes. I'd like to have employee and customer type to keep it simpler.)
</commit_message>
<xml_diff>
--- a/src/main/java/com/thewalking/shop/Product-inventory.xlsx
+++ b/src/main/java/com/thewalking/shop/Product-inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serka\Documents\CogentTheWalking\shop\shop\src\main\java\com\thewalking\shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70262E98-A447-40D3-8A63-45D45FDAD5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F63B24-BB04-409F-AC89-2CC934253B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="163">
   <si>
     <t>product</t>
   </si>
@@ -459,9 +459,6 @@
   </si>
   <si>
     <t>M - Check availability</t>
-  </si>
-  <si>
-    <t>O stock details: see total numbers one branch or all branches together at a time</t>
   </si>
   <si>
     <t>O - email service: give direct order to manufacturer and see requests from managers</t>
@@ -689,6 +686,34 @@
   </si>
   <si>
     <t>{{base}}/stocks/report/counts</t>
+  </si>
+  <si>
+    <t>{
+    "quantityRequested": 100,
+    "status": false,
+    "manager": {
+        "id":9
+    },
+    "owner": null,
+    "stock": {
+        "id": 8
+    }
+}</t>
+  </si>
+  <si>
+    <t>O stock details: see total numbers for all branches together at a time</t>
+  </si>
+  <si>
+    <t>O stock details: see total numbers for one branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{base}}/stockrequests
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{base}}/stockrequests
+*However, the manager should create the productDescription(if not exists), then the product(if not exists), then the stock with quantity of zero to claim a new design. All these entries contain enough information to convince the big BOSS*
+</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612DC713-9A32-4A78-A9EA-0C7C8E8F876A}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1349,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1342,12 +1367,12 @@
         <v>103</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,10 +1385,10 @@
         <v>105</v>
       </c>
       <c r="B12" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="156.75" x14ac:dyDescent="0.25">
@@ -1371,10 +1396,10 @@
         <v>106</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="206.25" x14ac:dyDescent="0.25">
@@ -1382,10 +1407,10 @@
         <v>107</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>142</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="206.25" x14ac:dyDescent="0.25">
@@ -1393,10 +1418,10 @@
         <v>108</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,10 +1443,10 @@
         <v>111</v>
       </c>
       <c r="B18" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,41 +1456,41 @@
     </row>
     <row r="23" spans="1:3" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>145</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>152</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>153</v>
       </c>
       <c r="C26" s="29"/>
     </row>
@@ -1474,147 +1499,182 @@
         <v>113</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="90.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>114</v>
+      <c r="A32" s="27" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B33" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="28" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="26" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>158</v>
-      </c>
       <c r="C34" s="28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>115</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B35" s="30"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="25" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>151</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
-        <v>122</v>
+      <c r="A44" s="27" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="27" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="27" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
search methods has been added to the stock service
</commit_message>
<xml_diff>
--- a/src/main/java/com/thewalking/shop/Product-inventory.xlsx
+++ b/src/main/java/com/thewalking/shop/Product-inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serka\Documents\CogentTheWalking\shop\shop\src\main\java\com\thewalking\shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F63B24-BB04-409F-AC89-2CC934253B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5FE4EC-9CBC-4AF0-AD09-C5375BBD06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="164">
   <si>
     <t>product</t>
   </si>
@@ -412,9 +412,6 @@
     <t xml:space="preserve">O M - Check Reviews </t>
   </si>
   <si>
-    <t>C - provide feedback to company. An email should be sent to customer to acknowledge the delivery</t>
-  </si>
-  <si>
     <t>O M - Respond to customer who left a feedback for the company</t>
   </si>
   <si>
@@ -513,15 +510,6 @@
   </si>
   <si>
     <t>M - check and reply feedbacks</t>
-  </si>
-  <si>
-    <t>O M - Can add edit categories</t>
-  </si>
-  <si>
-    <t>O M - Can add edit manufacturers</t>
-  </si>
-  <si>
-    <t>Manufacturers</t>
   </si>
   <si>
     <t>{{base}}/customers/signup</t>
@@ -664,9 +652,6 @@
     <t xml:space="preserve"> M O - Edit Product Details</t>
   </si>
   <si>
-    <t>All - Search product with SKU Code</t>
-  </si>
-  <si>
     <t>All - Search product details with product title, key words, categoryList</t>
   </si>
   <si>
@@ -714,6 +699,24 @@
     <t xml:space="preserve">{{base}}/stockrequests
 *However, the manager should create the productDescription(if not exists), then the product(if not exists), then the stock with quantity of zero to claim a new design. All these entries contain enough information to convince the big BOSS*
 </t>
+  </si>
+  <si>
+    <t>{{base}}/stocks/offers</t>
+  </si>
+  <si>
+    <t>All - Search products with TITLE, KEYWORS, and CATEGORY</t>
+  </si>
+  <si>
+    <t>{{base}}/reviews/company/all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C - provide feedback to company. </t>
+  </si>
+  <si>
+    <t>C - An email should be sent to customer to acknowledge the delivery of review</t>
+  </si>
+  <si>
+    <t>{{base}}/reviews</t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612DC713-9A32-4A78-A9EA-0C7C8E8F876A}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,345 +1339,362 @@
     <col min="5" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="206.25" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="206.25" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="132" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="29" t="s">
+      <c r="C5" s="29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+    </row>
+    <row r="8" spans="1:3" ht="132" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="29" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="26" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="206.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="29"/>
+    </row>
+    <row r="15" spans="1:3" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="206.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="29"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-    </row>
-    <row r="18" spans="1:3" ht="132" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>139</v>
+        <v>112</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="90.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="29"/>
-    </row>
-    <row r="25" spans="1:3" ht="123.75" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="B25" s="30"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="29"/>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="90.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>158</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="30"/>
+        <v>124</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>121</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
-        <v>127</v>
-      </c>
+      <c r="A47" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>